<commit_message>
complete  working income component
</commit_message>
<xml_diff>
--- a/server/incomes.details.xlsx
+++ b/server/incomes.details.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Incomes" sheetId="1" r:id="rId1"/>
+    <sheet name="Income" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,13 +397,210 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Icon</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Source</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Amount</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Date</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>📊</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Consulting</v>
+      </c>
+      <c r="C2">
+        <v>20000</v>
+      </c>
+      <c r="D2" t="str">
+        <v>24 Jul 2025</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>📝</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Content Writing</v>
+      </c>
+      <c r="C3">
+        <v>6200</v>
+      </c>
+      <c r="D3" t="str">
+        <v>23 Jul 2025</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>📦</v>
+      </c>
+      <c r="B4" t="str">
+        <v>E-commerce Sales</v>
+      </c>
+      <c r="C4">
+        <v>9500</v>
+      </c>
+      <c r="D4" t="str">
+        <v>22 Jul 2025</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>💰</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Side Hustle</v>
+      </c>
+      <c r="C5">
+        <v>5200</v>
+      </c>
+      <c r="D5" t="str">
+        <v>21 Jul 2025</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>💻</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Web Development</v>
+      </c>
+      <c r="C6">
+        <v>15000</v>
+      </c>
+      <c r="D6" t="str">
+        <v>20 Jul 2025</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>🎮</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Game Development</v>
+      </c>
+      <c r="C7">
+        <v>13000</v>
+      </c>
+      <c r="D7" t="str">
+        <v>19 Jul 2025</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>😃</v>
+      </c>
+      <c r="B8" t="str">
+        <v>freelance</v>
+      </c>
+      <c r="C8">
+        <v>15000</v>
+      </c>
+      <c r="D8" t="str">
+        <v>19 Jul 2025</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>💰</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Investments</v>
+      </c>
+      <c r="C9">
+        <v>9500</v>
+      </c>
+      <c r="D9" t="str">
+        <v>18 Jul 2025</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>🎓</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Online Tutoring</v>
+      </c>
+      <c r="C10">
+        <v>7400</v>
+      </c>
+      <c r="D10" t="str">
+        <v>18 Jul 2025</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>📸</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Photography</v>
+      </c>
+      <c r="C11">
+        <v>11200</v>
+      </c>
+      <c r="D11" t="str">
+        <v>17 Jul 2025</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>💰</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Bonus</v>
+      </c>
+      <c r="C12">
+        <v>8000</v>
+      </c>
+      <c r="D12" t="str">
+        <v>15 Jul 2025</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>🏟️</v>
+      </c>
+      <c r="B13" t="str">
+        <v>salary</v>
+      </c>
+      <c r="C13">
+        <v>40000</v>
+      </c>
+      <c r="D13" t="str">
+        <v>15 Jul 2025</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>💰</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Salary</v>
+      </c>
+      <c r="C14">
+        <v>45000</v>
+      </c>
+      <c r="D14" t="str">
+        <v>01 Jul 2025</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D14"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>